<commit_message>
update free asset list in documenation
</commit_message>
<xml_diff>
--- a/Documentation/Free_Assets_List.xlsx
+++ b/Documentation/Free_Assets_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natha\Unity Projects\3DPartyGame\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Projects\3DPartyGame\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51847A96-0BAB-4522-8E93-3D70818626C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9FBAB69-E157-4094-944B-A9E02239764F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,30 @@
   </si>
   <si>
     <t>Makes input handling easier to implement</t>
+  </si>
+  <si>
+    <t>Male Locomotion Animation Pack</t>
+  </si>
+  <si>
+    <t>Y Bot Model</t>
+  </si>
+  <si>
+    <t>Mixamo</t>
+  </si>
+  <si>
+    <t>Adobe Terms of Use (Free for video game use)</t>
+  </si>
+  <si>
+    <t>3D Model(s)</t>
+  </si>
+  <si>
+    <t>Animation(s)</t>
+  </si>
+  <si>
+    <t>3D Model we are using for our player character</t>
+  </si>
+  <si>
+    <t>Animations for our player character</t>
   </si>
 </sst>
 </file>
@@ -114,11 +138,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -131,25 +152,25 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -165,15 +186,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF8B9240-CDC3-4780-855D-D0702FD83D24}" name="Table1" displayName="Table1" ref="A1:F1048576" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FF8B9240-CDC3-4780-855D-D0702FD83D24}" name="Table1" displayName="Table1" ref="A1:F1048576" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <autoFilter ref="A1:F1048576" xr:uid="{FF8B9240-CDC3-4780-855D-D0702FD83D24}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2838FB65-3781-4AB7-BED5-AF59028582DD}" name="Name" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{6283AF30-C851-41D7-B01F-FAE7C28A212F}" name="Pack Name" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{1CE7DC97-5E26-4D43-93AA-C991C78BA560}" name="Source Name" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{BB92C8E0-D5F7-405B-96A8-7AC5083680DB}" name="License" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{1B8BAD52-0F80-4E28-B955-6CA6CFC7EEA1}" name="Type" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{1F075880-8DDB-4180-86CA-3948DCAB5096}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2838FB65-3781-4AB7-BED5-AF59028582DD}" name="Name" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{6283AF30-C851-41D7-B01F-FAE7C28A212F}" name="Pack Name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{1CE7DC97-5E26-4D43-93AA-C991C78BA560}" name="Source Name" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{BB92C8E0-D5F7-405B-96A8-7AC5083680DB}" name="License" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{1B8BAD52-0F80-4E28-B955-6CA6CFC7EEA1}" name="Type" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{1F075880-8DDB-4180-86CA-3948DCAB5096}" name="Description" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -442,23 +463,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.77734375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,11 +495,11 @@
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -494,11 +515,11 @@
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -514,11 +535,11 @@
       <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -534,8 +555,48 @@
       <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>